<commit_message>
some fixes in excel import
</commit_message>
<xml_diff>
--- a/Assets/Files/test.xlsx
+++ b/Assets/Files/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CodeConcept01\source\repos\DataImporter\Data-Importer\Assets\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F72B3EC-4918-43A7-88F6-DDBD598A74C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19D2DFD-6651-4335-88D5-B03D7715B4F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>variable 1</t>
   </si>
@@ -29,14 +29,26 @@
   </si>
   <si>
     <t>variable 3</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>08.02.2018 13:34:20</t>
+  </si>
+  <si>
+    <t>08.02.2018 13:34:30</t>
+  </si>
+  <si>
+    <t>08.02.2018 13:34:40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -66,9 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -450,87 +463,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="4" width="13" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
         <v>0.1011991198</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>0.47661715440000002</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.8710178677</v>
       </c>
       <c r="D2" s="1">
         <v>0.8710178677</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
         <v>9.9454306300000003E-2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>0.83527920300000003</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.50276619519999999</v>
       </c>
       <c r="D3" s="1">
         <v>0.50276619519999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
         <v>0.53904399950000004</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>0.66691643860000005</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.21445924299999999</v>
       </c>
       <c r="D4" s="1">
         <v>0.21445924299999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0.43024890030000001</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.6193666499999999E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.30826527110000002</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.30826527110000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>